<commit_message>
Sp carbon function update
</commit_message>
<xml_diff>
--- a/carbon_conversion_factors.xlsx
+++ b/carbon_conversion_factors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farne\Documents\Borealis_Ecological_Services\BVRC_20-37_TreeRecruitmentAfterFire\Data\Carbon conversion factors\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farne\Documents\Borealis_Ecological_Services\BVRC_20-37_TreeRecruitmentAfterFire\R_Scripts\Carbon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8028F16-2043-409C-AC41-DDEFF36B8C6E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905C1F42-BDE9-496C-B0CB-1CBB89BC84EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2364" yWindow="0" windowWidth="20676" windowHeight="12360" xr2:uid="{56A68C52-DBCB-4610-B458-EE2FDC1C347D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{56A68C52-DBCB-4610-B458-EE2FDC1C347D}"/>
   </bookViews>
   <sheets>
     <sheet name="CWD" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="79">
   <si>
     <t>Species</t>
   </si>
@@ -230,6 +230,48 @@
   </si>
   <si>
     <t>Unknown species</t>
+  </si>
+  <si>
+    <t>Updated:</t>
+  </si>
+  <si>
+    <t>Amabilis fir</t>
+  </si>
+  <si>
+    <t>Abies amabilis</t>
+  </si>
+  <si>
+    <t>Western hemlock</t>
+  </si>
+  <si>
+    <t>Tsuga heterophylla</t>
+  </si>
+  <si>
+    <t>Western red cedar</t>
+  </si>
+  <si>
+    <t>Thuja plicata</t>
+  </si>
+  <si>
+    <t>Douglas fir</t>
+  </si>
+  <si>
+    <t>Western larch</t>
+  </si>
+  <si>
+    <t>Larix occidentalis</t>
+  </si>
+  <si>
+    <t>Red alder</t>
+  </si>
+  <si>
+    <t>Alnus rubra</t>
+  </si>
+  <si>
+    <t>Pseudotsuga menziesii</t>
+  </si>
+  <si>
+    <t>(from gymnosperm whole-stem carbon conc)</t>
   </si>
 </sst>
 </file>
@@ -390,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -435,18 +477,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -761,42 +807,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F0CE288-C752-4EC8-BA98-6BD3D46E7E76}">
-  <dimension ref="A1:I89"/>
+  <dimension ref="A1:I125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.21875" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1796875" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" customWidth="1"/>
+    <col min="3" max="3" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" customWidth="1"/>
+    <col min="6" max="6" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>44235</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="2">
+        <v>44887</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
@@ -819,7 +868,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>3</v>
       </c>
@@ -842,7 +891,7 @@
         <v>0.49299999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7">
@@ -861,7 +910,7 @@
         <v>0.498</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7">
@@ -880,7 +929,7 @@
         <v>0.501</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7">
@@ -899,7 +948,7 @@
         <v>0.498</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7">
@@ -918,7 +967,7 @@
         <v>0.501</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="9"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10">
@@ -937,7 +986,7 @@
         <v>0.52100000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>12</v>
       </c>
@@ -960,7 +1009,7 @@
         <v>0.49299999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7">
@@ -979,7 +1028,7 @@
         <v>0.496</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7">
@@ -998,7 +1047,7 @@
         <v>0.498</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7">
@@ -1017,7 +1066,7 @@
         <v>0.505</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7">
@@ -1036,7 +1085,7 @@
         <v>0.52700000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10">
@@ -1055,7 +1104,7 @@
         <v>0.53500000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
         <v>13</v>
       </c>
@@ -1078,7 +1127,7 @@
         <v>0.49299999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="6"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7">
@@ -1097,7 +1146,7 @@
         <v>0.496</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7">
@@ -1116,7 +1165,7 @@
         <v>0.498</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7">
@@ -1135,7 +1184,7 @@
         <v>0.505</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="6"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7">
@@ -1154,7 +1203,7 @@
         <v>0.52100000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10">
@@ -1173,7 +1222,7 @@
         <v>0.53500000000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
         <v>28</v>
       </c>
@@ -1198,7 +1247,7 @@
         <v>0.49299999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="6"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7">
@@ -1219,7 +1268,7 @@
         <v>0.496</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="6"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7">
@@ -1240,7 +1289,7 @@
         <v>0.498</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="6"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7">
@@ -1261,7 +1310,7 @@
         <v>0.505</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="6"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7">
@@ -1282,7 +1331,7 @@
         <v>0.52100000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="9"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10">
@@ -1303,7 +1352,7 @@
         <v>0.53500000000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="12" t="s">
         <v>14</v>
       </c>
@@ -1326,7 +1375,7 @@
         <v>0.49299999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="6"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7">
@@ -1345,7 +1394,7 @@
         <v>0.497</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="6"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7">
@@ -1364,7 +1413,7 @@
         <v>0.496</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="6"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7">
@@ -1383,7 +1432,7 @@
         <v>0.499</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="6"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7">
@@ -1402,7 +1451,7 @@
         <v>0.51900000000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="9"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10">
@@ -1421,253 +1470,262 @@
         <v>0.52600000000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="12" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="C36" s="13">
         <v>0</v>
       </c>
       <c r="D36" s="13">
-        <v>0.48</v>
+        <v>0.4</v>
       </c>
       <c r="E36" s="13">
-        <v>0.48</v>
+        <v>0.4</v>
       </c>
       <c r="F36" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="G36" s="8">
-        <v>0.47199999999999998</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G36" s="14">
+        <v>0.48499999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="6"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7">
         <v>1</v>
       </c>
-      <c r="D37" s="7">
-        <v>0.46899999999999997</v>
-      </c>
-      <c r="E37" s="7">
-        <v>0.97699999999999998</v>
+      <c r="D37" s="15">
+        <v>0.36</v>
+      </c>
+      <c r="E37" s="15">
+        <v>0.9</v>
       </c>
       <c r="F37" s="7">
         <v>1</v>
       </c>
       <c r="G37" s="8">
-        <v>0.47799999999999998</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.48699999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="6"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7">
         <v>2</v>
       </c>
-      <c r="D38" s="7">
-        <v>0.40300000000000002</v>
-      </c>
-      <c r="E38" s="7">
-        <v>0.66</v>
+      <c r="D38" s="15">
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="E38" s="15">
+        <v>0.83</v>
       </c>
       <c r="F38" s="7">
         <v>1</v>
       </c>
       <c r="G38" s="8">
-        <v>0.47699999999999998</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.48499999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="6"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7">
         <v>3</v>
       </c>
-      <c r="D39" s="7">
-        <v>0.35199999999999998</v>
-      </c>
-      <c r="E39" s="7">
-        <v>0.73299999999999998</v>
+      <c r="D39" s="15">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="E39" s="15">
+        <v>0.60399999999999998</v>
       </c>
       <c r="F39" s="7">
         <v>1</v>
       </c>
       <c r="G39" s="8">
-        <v>0.48099999999999998</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.505</v>
+      </c>
+      <c r="H39" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="6"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7">
         <v>4</v>
       </c>
-      <c r="D40" s="7">
-        <v>0.17</v>
-      </c>
-      <c r="E40" s="7">
-        <v>0.309</v>
+      <c r="D40" s="15">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="E40" s="15">
+        <v>0.40400000000000003</v>
       </c>
       <c r="F40" s="7">
         <v>0.8</v>
       </c>
       <c r="G40" s="8">
-        <v>0.47399999999999998</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="H40" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="9"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10">
         <v>5</v>
       </c>
       <c r="D41" s="10">
-        <v>0.11</v>
+        <v>0.106</v>
       </c>
       <c r="E41" s="10">
-        <v>0.2</v>
+        <v>0.309</v>
       </c>
       <c r="F41" s="10">
         <v>0.41199999999999998</v>
       </c>
-      <c r="G41" s="8">
-        <v>0.47299999999999998</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G41" s="11">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="H41" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="12" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="C42" s="13">
         <v>0</v>
       </c>
-      <c r="D42" s="13">
-        <v>0.35</v>
-      </c>
-      <c r="E42" s="13">
-        <v>0.35</v>
+      <c r="D42" s="15">
+        <v>0.42</v>
+      </c>
+      <c r="E42" s="15">
+        <v>0.42</v>
       </c>
       <c r="F42" s="13" t="s">
         <v>21</v>
       </c>
       <c r="G42" s="14">
-        <v>0.47199999999999998</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.48599999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="6"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7">
         <v>1</v>
       </c>
-      <c r="D43" s="7">
-        <v>0.35299999999999998</v>
-      </c>
-      <c r="E43" s="7">
-        <v>0.96699999999999997</v>
+      <c r="D43" s="15">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="E43" s="15">
+        <v>0.89</v>
       </c>
       <c r="F43" s="7">
         <v>1</v>
       </c>
       <c r="G43" s="8">
-        <v>0.48799999999999999</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.48399999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="6"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7">
         <v>2</v>
       </c>
-      <c r="D44" s="7">
-        <v>0.42199999999999999</v>
-      </c>
-      <c r="E44" s="7">
-        <v>0.73399999999999999</v>
+      <c r="D44" s="15">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="E44" s="15">
+        <v>0.76700000000000002</v>
       </c>
       <c r="F44" s="7">
         <v>1</v>
       </c>
       <c r="G44" s="8">
-        <v>0.48899999999999999</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.498</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="6"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7">
         <v>3</v>
       </c>
-      <c r="D45" s="7">
-        <v>0.29899999999999999</v>
-      </c>
-      <c r="E45" s="7">
-        <v>0.81899999999999995</v>
+      <c r="D45" s="15">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="E45" s="15">
+        <v>0.63600000000000001</v>
       </c>
       <c r="F45" s="7">
         <v>1</v>
       </c>
       <c r="G45" s="8">
-        <v>0.495</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.51500000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="6"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7">
         <v>4</v>
       </c>
-      <c r="D46" s="7">
-        <v>0.16</v>
-      </c>
-      <c r="E46" s="7">
-        <v>0.432</v>
+      <c r="D46" s="15">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="E46" s="15">
+        <v>0.42499999999999999</v>
       </c>
       <c r="F46" s="7">
         <v>0.8</v>
       </c>
       <c r="G46" s="8">
-        <v>0.46500000000000002</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.53400000000000003</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="9"/>
       <c r="B47" s="10"/>
       <c r="C47" s="10">
         <v>5</v>
       </c>
       <c r="D47" s="10">
-        <v>0.11</v>
+        <v>0.108</v>
       </c>
       <c r="E47" s="10">
-        <v>0.29699999999999999</v>
+        <v>0.33200000000000002</v>
       </c>
       <c r="F47" s="10">
         <v>0.41199999999999998</v>
       </c>
       <c r="G47" s="11">
-        <v>0.47299999999999998</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="12" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="C48" s="13">
         <v>0</v>
       </c>
-      <c r="D48" s="13">
+      <c r="D48">
         <v>0.31</v>
       </c>
       <c r="E48" s="13">
@@ -1676,639 +1734,1380 @@
       <c r="F48" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="G48" s="8">
-        <v>0.47199999999999998</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G48" s="14">
+        <v>0.49299999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="6"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7">
         <v>1</v>
       </c>
-      <c r="D49" s="7">
-        <v>0.35299999999999998</v>
+      <c r="D49">
+        <v>0.318</v>
       </c>
       <c r="E49" s="7">
-        <v>0.96699999999999997</v>
+        <v>1</v>
       </c>
       <c r="F49" s="7">
         <v>1</v>
       </c>
       <c r="G49" s="8">
-        <v>0.47799999999999998</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.496</v>
+      </c>
+      <c r="H49" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="6"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7">
         <v>2</v>
       </c>
-      <c r="D50" s="7">
-        <v>0.42199999999999999</v>
+      <c r="D50">
+        <v>0.25900000000000001</v>
       </c>
       <c r="E50" s="7">
-        <v>0.73399999999999999</v>
+        <v>0.83499999999999996</v>
       </c>
       <c r="F50" s="7">
         <v>1</v>
       </c>
       <c r="G50" s="8">
-        <v>0.47699999999999998</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.498</v>
+      </c>
+      <c r="H50" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="6"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7">
         <v>3</v>
       </c>
-      <c r="D51" s="7">
-        <v>0.29899999999999999</v>
-      </c>
-      <c r="E51" s="7">
-        <v>0.81899999999999995</v>
+      <c r="D51">
+        <v>0.248</v>
+      </c>
+      <c r="E51" s="15">
+        <v>0.8</v>
       </c>
       <c r="F51" s="7">
         <v>1</v>
       </c>
       <c r="G51" s="8">
-        <v>0.48099999999999998</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.505</v>
+      </c>
+      <c r="H51" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="6"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7">
         <v>4</v>
       </c>
-      <c r="D52" s="7">
-        <v>0.16</v>
-      </c>
-      <c r="E52" s="7">
-        <v>0.432</v>
+      <c r="D52">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="E52" s="15">
+        <v>0.46200000000000002</v>
       </c>
       <c r="F52" s="7">
         <v>0.8</v>
       </c>
       <c r="G52" s="8">
-        <v>0.47399999999999998</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="H52" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="9"/>
       <c r="B53" s="10"/>
       <c r="C53" s="10">
         <v>5</v>
       </c>
-      <c r="D53" s="10">
-        <v>0.11</v>
+      <c r="D53">
+        <v>0.14299999999999999</v>
       </c>
       <c r="E53" s="10">
-        <v>0.29699999999999999</v>
+        <v>0.46100000000000002</v>
       </c>
       <c r="F53" s="10">
         <v>0.41199999999999998</v>
       </c>
       <c r="G53" s="11">
-        <v>0.47299999999999998</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="H53" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="12" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="C54" s="13">
         <v>0</v>
       </c>
       <c r="D54" s="13">
-        <f>AVERAGE(D6,D24,D30)</f>
-        <v>0.34666666666666668</v>
+        <v>0.45</v>
       </c>
       <c r="E54" s="13">
-        <f>AVERAGE(E6,E24,E30)</f>
-        <v>0.34666666666666668</v>
+        <v>0.45</v>
       </c>
       <c r="F54" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="G54" s="8">
-        <v>0.49299999999999999</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G54" s="14">
+        <v>0.48899999999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="6"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7">
         <v>1</v>
       </c>
-      <c r="D55" s="7">
-        <f t="shared" ref="D55:E59" si="1">AVERAGE(D7,D25,D31)</f>
-        <v>0.38066666666666665</v>
+      <c r="D55">
+        <v>0.38600000000000001</v>
       </c>
       <c r="E55" s="7">
-        <f t="shared" si="1"/>
-        <v>0.97800000000000009</v>
+        <v>0.85799999999999998</v>
       </c>
       <c r="F55" s="7">
         <v>1</v>
       </c>
       <c r="G55" s="8">
-        <v>0.496</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.48799999999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="6"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7">
         <v>2</v>
       </c>
       <c r="D56" s="7">
-        <f t="shared" si="1"/>
-        <v>0.3133333333333333</v>
+        <v>0.308</v>
       </c>
       <c r="E56" s="7">
-        <f t="shared" si="1"/>
-        <v>0.90166666666666673</v>
+        <v>0.72299999999999998</v>
       </c>
       <c r="F56" s="7">
         <v>1</v>
       </c>
       <c r="G56" s="8">
-        <v>0.498</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.499</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="6"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7">
         <v>3</v>
       </c>
       <c r="D57" s="7">
-        <f t="shared" si="1"/>
-        <v>0.26300000000000001</v>
-      </c>
-      <c r="E57" s="7">
-        <f t="shared" si="1"/>
-        <v>0.76866666666666672</v>
+        <v>0.152</v>
+      </c>
+      <c r="E57" s="15">
+        <v>0.44400000000000001</v>
       </c>
       <c r="F57" s="7">
         <v>1</v>
       </c>
       <c r="G57" s="8">
-        <v>0.505</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.495</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="6"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7">
         <v>4</v>
       </c>
-      <c r="D58" s="7">
-        <f t="shared" si="1"/>
-        <v>0.15233333333333335</v>
-      </c>
-      <c r="E58" s="7">
-        <f t="shared" si="1"/>
-        <v>0.46416666666666667</v>
+      <c r="D58" s="15">
+        <v>0.123</v>
+      </c>
+      <c r="E58" s="15">
+        <v>0.30499999999999999</v>
       </c>
       <c r="F58" s="7">
         <v>0.8</v>
       </c>
       <c r="G58" s="8">
-        <v>0.52100000000000002</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.53900000000000003</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="9"/>
       <c r="B59" s="10"/>
       <c r="C59" s="10">
         <v>5</v>
       </c>
-      <c r="D59" s="10">
-        <f t="shared" si="1"/>
-        <v>0.13666666666666669</v>
+      <c r="D59" s="43">
+        <v>0.14799999999999999</v>
       </c>
       <c r="E59" s="10">
-        <f t="shared" si="1"/>
-        <v>0.26333333333333336</v>
+        <v>0.32900000000000001</v>
       </c>
       <c r="F59" s="10">
         <v>0.41199999999999998</v>
       </c>
       <c r="G59" s="11">
-        <v>0.53500000000000003</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.55800000000000005</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" s="12" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="C60" s="13">
         <v>0</v>
       </c>
       <c r="D60" s="13">
-        <f>AVERAGE(D48,D42,D36)</f>
-        <v>0.37999999999999995</v>
+        <v>0.48</v>
       </c>
       <c r="E60" s="13">
-        <f>AVERAGE(E48,E42,E36)</f>
-        <v>0.37999999999999995</v>
+        <v>0.48</v>
       </c>
       <c r="F60" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="G60" s="8">
-        <v>0.47199999999999998</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G60" s="14">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="H60" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="6"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7">
         <v>1</v>
       </c>
-      <c r="D61" s="7">
-        <f>AVERAGE(D49,D43,D37)</f>
-        <v>0.39166666666666661</v>
+      <c r="D61" s="15">
+        <v>0.38100000000000001</v>
       </c>
       <c r="E61" s="7">
-        <f t="shared" ref="E61:E65" si="2">AVERAGE(E49,E43,E37)</f>
-        <v>0.97033333333333338</v>
+        <v>0.95599999999999996</v>
       </c>
       <c r="F61" s="7">
         <v>1</v>
       </c>
       <c r="G61" s="8">
-        <v>0.47799999999999998</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.496</v>
+      </c>
+      <c r="H61" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="6"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7">
         <v>2</v>
       </c>
-      <c r="D62" s="7">
-        <f>AVERAGE(D50,D44,D38)</f>
-        <v>0.41566666666666663</v>
+      <c r="D62" s="15">
+        <v>0.318</v>
       </c>
       <c r="E62" s="7">
-        <f t="shared" si="2"/>
-        <v>0.70933333333333337</v>
+        <v>0.82699999999999996</v>
       </c>
       <c r="F62" s="7">
         <v>1</v>
       </c>
       <c r="G62" s="8">
-        <v>0.47699999999999998</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.498</v>
+      </c>
+      <c r="H62" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="6"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7">
         <v>3</v>
       </c>
-      <c r="D63" s="7">
-        <f>AVERAGE(D51,D45,D39)</f>
-        <v>0.31666666666666665</v>
-      </c>
-      <c r="E63" s="7">
-        <f t="shared" si="2"/>
-        <v>0.79033333333333333</v>
+      <c r="D63" s="15">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="E63" s="15">
+        <v>0.67800000000000005</v>
       </c>
       <c r="F63" s="7">
         <v>1</v>
       </c>
       <c r="G63" s="8">
-        <v>0.48099999999999998</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.505</v>
+      </c>
+      <c r="H63" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="6"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7">
         <v>4</v>
       </c>
-      <c r="D64" s="7">
-        <f>AVERAGE(D52,D46,D40)</f>
-        <v>0.16333333333333333</v>
-      </c>
-      <c r="E64" s="7">
-        <f t="shared" si="2"/>
-        <v>0.39100000000000001</v>
+      <c r="D64" s="15">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="E64" s="15">
+        <v>0.42599999999999999</v>
       </c>
       <c r="F64" s="7">
         <v>0.8</v>
       </c>
       <c r="G64" s="8">
-        <v>0.47399999999999998</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="H64" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="9"/>
       <c r="B65" s="10"/>
       <c r="C65" s="10">
         <v>5</v>
       </c>
       <c r="D65" s="10">
-        <f t="shared" ref="D65" si="3">AVERAGE(D53,D47,D41)</f>
-        <v>0.11</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="E65" s="10">
-        <f t="shared" si="2"/>
-        <v>0.26466666666666666</v>
+        <v>0.36599999999999999</v>
       </c>
       <c r="F65" s="10">
         <v>0.41199999999999998</v>
       </c>
       <c r="G65" s="11">
-        <v>0.47299999999999998</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C66" s="7">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="H65" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A66" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B66" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C66" s="13">
         <v>0</v>
       </c>
-      <c r="D66" s="7">
-        <f t="shared" ref="D66:D71" si="4">AVERAGE(D48,D42,D36,D30,D24,D6)</f>
-        <v>0.36333333333333334</v>
-      </c>
-      <c r="E66" s="7">
-        <f>AVERAGE(E6,E24,E30,E36,E42,E48)</f>
-        <v>0.36333333333333334</v>
-      </c>
-      <c r="F66" s="7" t="s">
+      <c r="D66" s="13">
+        <v>0.48</v>
+      </c>
+      <c r="E66" s="13">
+        <v>0.48</v>
+      </c>
+      <c r="F66" s="13" t="s">
         <v>21</v>
       </c>
       <c r="G66" s="8">
-        <f>AVERAGE(G54,G60)</f>
-        <v>0.48249999999999998</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.47199999999999998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="6"/>
       <c r="B67" s="7"/>
       <c r="C67" s="7">
         <v>1</v>
       </c>
       <c r="D67" s="7">
-        <f t="shared" si="4"/>
-        <v>0.38616666666666671</v>
+        <v>0.46899999999999997</v>
       </c>
       <c r="E67" s="7">
-        <f>AVERAGE(E7,E25,E31,E37,E43,E49)</f>
-        <v>0.97416666666666663</v>
+        <v>0.97699999999999998</v>
       </c>
       <c r="F67" s="7">
         <v>1</v>
       </c>
       <c r="G67" s="8">
-        <f t="shared" ref="G67:G71" si="5">AVERAGE(G55,G61)</f>
-        <v>0.48699999999999999</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.47799999999999998</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" s="6"/>
       <c r="B68" s="7"/>
       <c r="C68" s="7">
         <v>2</v>
       </c>
       <c r="D68" s="7">
-        <f t="shared" si="4"/>
-        <v>0.36449999999999999</v>
+        <v>0.40300000000000002</v>
       </c>
       <c r="E68" s="7">
-        <f t="shared" ref="E68:E71" si="6">AVERAGE(E8,E26,E32,E38,E44,E50)</f>
-        <v>0.80549999999999999</v>
+        <v>0.66</v>
       </c>
       <c r="F68" s="7">
         <v>1</v>
       </c>
       <c r="G68" s="8">
-        <f t="shared" si="5"/>
-        <v>0.48749999999999999</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.47699999999999998</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" s="6"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7">
         <v>3</v>
       </c>
       <c r="D69" s="7">
-        <f t="shared" si="4"/>
-        <v>0.28983333333333333</v>
+        <v>0.35199999999999998</v>
       </c>
       <c r="E69" s="7">
-        <f t="shared" si="6"/>
-        <v>0.77949999999999997</v>
+        <v>0.73299999999999998</v>
       </c>
       <c r="F69" s="7">
         <v>1</v>
       </c>
       <c r="G69" s="8">
-        <f t="shared" si="5"/>
-        <v>0.49299999999999999</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.48099999999999998</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" s="6"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7">
         <v>4</v>
       </c>
       <c r="D70" s="7">
-        <f t="shared" si="4"/>
-        <v>0.15783333333333335</v>
+        <v>0.17</v>
       </c>
       <c r="E70" s="7">
-        <f t="shared" si="6"/>
-        <v>0.42758333333333337</v>
+        <v>0.309</v>
       </c>
       <c r="F70" s="7">
         <v>0.8</v>
       </c>
       <c r="G70" s="8">
-        <f t="shared" si="5"/>
-        <v>0.4975</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.47399999999999998</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" s="9"/>
       <c r="B71" s="10"/>
       <c r="C71" s="10">
         <v>5</v>
       </c>
       <c r="D71" s="10">
-        <f t="shared" si="4"/>
-        <v>0.12333333333333334</v>
+        <v>0.11</v>
       </c>
       <c r="E71" s="10">
-        <f t="shared" si="6"/>
-        <v>0.26399999999999996</v>
+        <v>0.2</v>
       </c>
       <c r="F71" s="10">
         <v>0.41199999999999998</v>
       </c>
-      <c r="G71" s="11">
-        <f t="shared" si="5"/>
+      <c r="G71" s="8">
+        <v>0.47299999999999998</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A72" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B72" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72" s="13">
+        <v>0</v>
+      </c>
+      <c r="D72" s="13">
+        <v>0.35</v>
+      </c>
+      <c r="E72" s="13">
+        <v>0.35</v>
+      </c>
+      <c r="F72" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G72" s="14">
+        <v>0.47199999999999998</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A73" s="6"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="7">
+        <v>1</v>
+      </c>
+      <c r="D73" s="7">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="E73" s="7">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="F73" s="7">
+        <v>1</v>
+      </c>
+      <c r="G73" s="8">
+        <v>0.48799999999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A74" s="6"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7">
+        <v>2</v>
+      </c>
+      <c r="D74" s="7">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="E74" s="7">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="F74" s="7">
+        <v>1</v>
+      </c>
+      <c r="G74" s="8">
+        <v>0.48899999999999999</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A75" s="6"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="7">
+        <v>3</v>
+      </c>
+      <c r="D75" s="7">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="E75" s="7">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="F75" s="7">
+        <v>1</v>
+      </c>
+      <c r="G75" s="8">
+        <v>0.495</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A76" s="6"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7">
+        <v>4</v>
+      </c>
+      <c r="D76" s="7">
+        <v>0.16</v>
+      </c>
+      <c r="E76" s="7">
+        <v>0.432</v>
+      </c>
+      <c r="F76" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="G76" s="8">
+        <v>0.46500000000000002</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A77" s="9"/>
+      <c r="B77" s="10"/>
+      <c r="C77" s="10">
+        <v>5</v>
+      </c>
+      <c r="D77" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="E77" s="10">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="F77" s="10">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="G77" s="11">
+        <v>0.47299999999999998</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A78" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B78" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C78" s="13">
+        <v>0</v>
+      </c>
+      <c r="D78" s="13">
+        <v>0.31</v>
+      </c>
+      <c r="E78" s="13">
+        <v>0.31</v>
+      </c>
+      <c r="F78" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G78" s="8">
+        <v>0.47199999999999998</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A79" s="6"/>
+      <c r="B79" s="7"/>
+      <c r="C79" s="7">
+        <v>1</v>
+      </c>
+      <c r="D79" s="7">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="E79" s="7">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="F79" s="7">
+        <v>1</v>
+      </c>
+      <c r="G79" s="8">
+        <v>0.47799999999999998</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A80" s="6"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="7">
+        <v>2</v>
+      </c>
+      <c r="D80" s="7">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="E80" s="7">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="F80" s="7">
+        <v>1</v>
+      </c>
+      <c r="G80" s="8">
+        <v>0.47699999999999998</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A81" s="6"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="7">
+        <v>3</v>
+      </c>
+      <c r="D81" s="7">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="E81" s="7">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="F81" s="7">
+        <v>1</v>
+      </c>
+      <c r="G81" s="8">
+        <v>0.48099999999999998</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A82" s="6"/>
+      <c r="B82" s="7"/>
+      <c r="C82" s="7">
+        <v>4</v>
+      </c>
+      <c r="D82" s="7">
+        <v>0.16</v>
+      </c>
+      <c r="E82" s="7">
+        <v>0.432</v>
+      </c>
+      <c r="F82" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="G82" s="8">
+        <v>0.47399999999999998</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A83" s="9"/>
+      <c r="B83" s="10"/>
+      <c r="C83" s="10">
+        <v>5</v>
+      </c>
+      <c r="D83" s="10">
+        <v>0.11</v>
+      </c>
+      <c r="E83" s="10">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="F83" s="10">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="G83" s="11">
+        <v>0.47299999999999998</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A84" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B84" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C84" s="13">
+        <v>0</v>
+      </c>
+      <c r="D84" s="13">
+        <v>0.37</v>
+      </c>
+      <c r="E84" s="13">
+        <v>0.37</v>
+      </c>
+      <c r="F84" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G84" s="15">
+        <v>0.48099999999999998</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A85" s="6"/>
+      <c r="B85" s="7"/>
+      <c r="C85" s="7">
+        <v>1</v>
+      </c>
+      <c r="D85" s="15">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="E85" s="15">
+        <v>0.99</v>
+      </c>
+      <c r="F85" s="7">
+        <v>1</v>
+      </c>
+      <c r="G85" s="8">
+        <v>0.48199999999999998</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A86" s="6"/>
+      <c r="B86" s="7"/>
+      <c r="C86" s="7">
+        <v>2</v>
+      </c>
+      <c r="D86" s="15">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="E86" s="15">
+        <v>0.83599999999999997</v>
+      </c>
+      <c r="F86" s="7">
+        <v>1</v>
+      </c>
+      <c r="G86" s="8">
+        <v>0.48099999999999998</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A87" s="6"/>
+      <c r="B87" s="7"/>
+      <c r="C87" s="7">
+        <v>3</v>
+      </c>
+      <c r="D87" s="15">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="E87" s="15">
+        <v>0.505</v>
+      </c>
+      <c r="F87" s="7">
+        <v>1</v>
+      </c>
+      <c r="G87" s="8">
+        <v>0.48199999999999998</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A88" s="6"/>
+      <c r="B88" s="7"/>
+      <c r="C88" s="7">
+        <v>4</v>
+      </c>
+      <c r="D88" s="15">
+        <v>0.108</v>
+      </c>
+      <c r="E88" s="15">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="F88" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="G88" s="8">
+        <v>0.49199999999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A89" s="9"/>
+      <c r="B89" s="10"/>
+      <c r="C89" s="10">
+        <v>5</v>
+      </c>
+      <c r="D89" s="10">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="E89" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="F89" s="10">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="G89" s="11">
+        <v>0.45500000000000002</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A90" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B90" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C90" s="13">
+        <v>0</v>
+      </c>
+      <c r="D90" s="13">
+        <f>AVERAGE(D6,D24,D30)</f>
+        <v>0.34666666666666668</v>
+      </c>
+      <c r="E90" s="13">
+        <f>AVERAGE(E6,E24,E30)</f>
+        <v>0.34666666666666668</v>
+      </c>
+      <c r="F90" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G90" s="8">
+        <v>0.49299999999999999</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A91" s="6"/>
+      <c r="B91" s="7"/>
+      <c r="C91" s="7">
+        <v>1</v>
+      </c>
+      <c r="D91" s="7">
+        <f>AVERAGE(D7,D25,D31)</f>
+        <v>0.38066666666666665</v>
+      </c>
+      <c r="E91" s="7">
+        <f>AVERAGE(E7,E25,E31)</f>
+        <v>0.97800000000000009</v>
+      </c>
+      <c r="F91" s="7">
+        <v>1</v>
+      </c>
+      <c r="G91" s="8">
+        <v>0.496</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A92" s="6"/>
+      <c r="B92" s="7"/>
+      <c r="C92" s="7">
+        <v>2</v>
+      </c>
+      <c r="D92" s="7">
+        <f>AVERAGE(D8,D26,D32)</f>
+        <v>0.3133333333333333</v>
+      </c>
+      <c r="E92" s="7">
+        <f>AVERAGE(E8,E26,E32)</f>
+        <v>0.90166666666666673</v>
+      </c>
+      <c r="F92" s="7">
+        <v>1</v>
+      </c>
+      <c r="G92" s="8">
+        <v>0.498</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A93" s="6"/>
+      <c r="B93" s="7"/>
+      <c r="C93" s="7">
+        <v>3</v>
+      </c>
+      <c r="D93" s="7">
+        <f>AVERAGE(D9,D27,D33)</f>
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="E93" s="7">
+        <f>AVERAGE(E9,E27,E33)</f>
+        <v>0.76866666666666672</v>
+      </c>
+      <c r="F93" s="7">
+        <v>1</v>
+      </c>
+      <c r="G93" s="8">
+        <v>0.505</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A94" s="6"/>
+      <c r="B94" s="7"/>
+      <c r="C94" s="7">
+        <v>4</v>
+      </c>
+      <c r="D94" s="7">
+        <f>AVERAGE(D10,D28,D34)</f>
+        <v>0.15233333333333335</v>
+      </c>
+      <c r="E94" s="7">
+        <f>AVERAGE(E10,E28,E34)</f>
+        <v>0.46416666666666667</v>
+      </c>
+      <c r="F94" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="G94" s="8">
+        <v>0.52100000000000002</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A95" s="9"/>
+      <c r="B95" s="10"/>
+      <c r="C95" s="10">
+        <v>5</v>
+      </c>
+      <c r="D95" s="10">
+        <f>AVERAGE(D11,D29,D35)</f>
+        <v>0.13666666666666669</v>
+      </c>
+      <c r="E95" s="10">
+        <f>AVERAGE(E11,E29,E35)</f>
+        <v>0.26333333333333336</v>
+      </c>
+      <c r="F95" s="10">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="G95" s="11">
+        <v>0.53500000000000003</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A96" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B96" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C96" s="13">
+        <v>0</v>
+      </c>
+      <c r="D96" s="13">
+        <f>AVERAGE(D78,D72,D66)</f>
+        <v>0.37999999999999995</v>
+      </c>
+      <c r="E96" s="13">
+        <f>AVERAGE(E78,E72,E66)</f>
+        <v>0.37999999999999995</v>
+      </c>
+      <c r="F96" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G96" s="8">
+        <v>0.47199999999999998</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A97" s="6"/>
+      <c r="B97" s="7"/>
+      <c r="C97" s="7">
+        <v>1</v>
+      </c>
+      <c r="D97" s="7">
+        <f>AVERAGE(D79,D73,D67)</f>
+        <v>0.39166666666666661</v>
+      </c>
+      <c r="E97" s="7">
+        <f>AVERAGE(E79,E73,E67)</f>
+        <v>0.97033333333333338</v>
+      </c>
+      <c r="F97" s="7">
+        <v>1</v>
+      </c>
+      <c r="G97" s="8">
+        <v>0.47799999999999998</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A98" s="6"/>
+      <c r="B98" s="7"/>
+      <c r="C98" s="7">
+        <v>2</v>
+      </c>
+      <c r="D98" s="7">
+        <f>AVERAGE(D80,D74,D68)</f>
+        <v>0.41566666666666663</v>
+      </c>
+      <c r="E98" s="7">
+        <f>AVERAGE(E80,E74,E68)</f>
+        <v>0.70933333333333337</v>
+      </c>
+      <c r="F98" s="7">
+        <v>1</v>
+      </c>
+      <c r="G98" s="8">
+        <v>0.47699999999999998</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A99" s="6"/>
+      <c r="B99" s="7"/>
+      <c r="C99" s="7">
+        <v>3</v>
+      </c>
+      <c r="D99" s="7">
+        <f>AVERAGE(D81,D75,D69)</f>
+        <v>0.31666666666666665</v>
+      </c>
+      <c r="E99" s="7">
+        <f>AVERAGE(E81,E75,E69)</f>
+        <v>0.79033333333333333</v>
+      </c>
+      <c r="F99" s="7">
+        <v>1</v>
+      </c>
+      <c r="G99" s="8">
+        <v>0.48099999999999998</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A100" s="6"/>
+      <c r="B100" s="7"/>
+      <c r="C100" s="7">
+        <v>4</v>
+      </c>
+      <c r="D100" s="7">
+        <f>AVERAGE(D82,D76,D70)</f>
+        <v>0.16333333333333333</v>
+      </c>
+      <c r="E100" s="7">
+        <f>AVERAGE(E82,E76,E70)</f>
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="F100" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="G100" s="8">
+        <v>0.47399999999999998</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A101" s="9"/>
+      <c r="B101" s="10"/>
+      <c r="C101" s="10">
+        <v>5</v>
+      </c>
+      <c r="D101" s="10">
+        <f t="shared" ref="D101" si="1">AVERAGE(D83,D77,D71)</f>
+        <v>0.11</v>
+      </c>
+      <c r="E101" s="10">
+        <f>AVERAGE(E83,E77,E71)</f>
+        <v>0.26466666666666666</v>
+      </c>
+      <c r="F101" s="10">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="G101" s="11">
+        <v>0.47299999999999998</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A102" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C102" s="7">
+        <v>0</v>
+      </c>
+      <c r="D102" s="7">
+        <f>AVERAGE(D78,D72,D66,D30,D24,D6)</f>
+        <v>0.36333333333333334</v>
+      </c>
+      <c r="E102" s="7">
+        <f>AVERAGE(E6,E24,E30,E66,E72,E78)</f>
+        <v>0.36333333333333334</v>
+      </c>
+      <c r="F102" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G102" s="8">
+        <f>AVERAGE(G90,G96)</f>
+        <v>0.48249999999999998</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A103" s="6"/>
+      <c r="B103" s="7"/>
+      <c r="C103" s="7">
+        <v>1</v>
+      </c>
+      <c r="D103" s="7">
+        <f>AVERAGE(D79,D73,D67,D31,D25,D7)</f>
+        <v>0.38616666666666671</v>
+      </c>
+      <c r="E103" s="7">
+        <f>AVERAGE(E7,E25,E31,E67,E73,E79)</f>
+        <v>0.97416666666666663</v>
+      </c>
+      <c r="F103" s="7">
+        <v>1</v>
+      </c>
+      <c r="G103" s="8">
+        <f t="shared" ref="G103:G107" si="2">AVERAGE(G91,G97)</f>
+        <v>0.48699999999999999</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A104" s="6"/>
+      <c r="B104" s="7"/>
+      <c r="C104" s="7">
+        <v>2</v>
+      </c>
+      <c r="D104" s="7">
+        <f>AVERAGE(D80,D74,D68,D32,D26,D8)</f>
+        <v>0.36449999999999999</v>
+      </c>
+      <c r="E104" s="7">
+        <f>AVERAGE(E8,E26,E32,E68,E74,E80)</f>
+        <v>0.80549999999999999</v>
+      </c>
+      <c r="F104" s="7">
+        <v>1</v>
+      </c>
+      <c r="G104" s="8">
+        <f t="shared" si="2"/>
+        <v>0.48749999999999999</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A105" s="6"/>
+      <c r="B105" s="7"/>
+      <c r="C105" s="7">
+        <v>3</v>
+      </c>
+      <c r="D105" s="7">
+        <f>AVERAGE(D81,D75,D69,D33,D27,D9)</f>
+        <v>0.28983333333333333</v>
+      </c>
+      <c r="E105" s="7">
+        <f>AVERAGE(E9,E27,E33,E69,E75,E81)</f>
+        <v>0.77949999999999997</v>
+      </c>
+      <c r="F105" s="7">
+        <v>1</v>
+      </c>
+      <c r="G105" s="8">
+        <f t="shared" si="2"/>
+        <v>0.49299999999999999</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A106" s="6"/>
+      <c r="B106" s="7"/>
+      <c r="C106" s="7">
+        <v>4</v>
+      </c>
+      <c r="D106" s="7">
+        <f>AVERAGE(D82,D76,D70,D34,D28,D10)</f>
+        <v>0.15783333333333335</v>
+      </c>
+      <c r="E106" s="7">
+        <f>AVERAGE(E10,E28,E34,E70,E76,E82)</f>
+        <v>0.42758333333333337</v>
+      </c>
+      <c r="F106" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="G106" s="8">
+        <f t="shared" si="2"/>
+        <v>0.4975</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A107" s="9"/>
+      <c r="B107" s="10"/>
+      <c r="C107" s="10">
+        <v>5</v>
+      </c>
+      <c r="D107" s="10">
+        <f>AVERAGE(D83,D77,D71,D35,D29,D11)</f>
+        <v>0.12333333333333334</v>
+      </c>
+      <c r="E107" s="10">
+        <f>AVERAGE(E11,E29,E35,E71,E77,E83)</f>
+        <v>0.26399999999999996</v>
+      </c>
+      <c r="F107" s="10">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="G107" s="11">
+        <f t="shared" si="2"/>
         <v>0.504</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" s="3" t="s">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A110" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B74" s="13"/>
-      <c r="C74" s="13"/>
-      <c r="D74" s="13"/>
-      <c r="E74" s="13"/>
-      <c r="F74" s="13"/>
-      <c r="G74" s="13"/>
-      <c r="H74" s="13"/>
-      <c r="I74" s="14"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75" s="6" t="s">
+      <c r="B110" s="13"/>
+      <c r="C110" s="13"/>
+      <c r="D110" s="13"/>
+      <c r="E110" s="13"/>
+      <c r="F110" s="13"/>
+      <c r="G110" s="13"/>
+      <c r="H110" s="13"/>
+      <c r="I110" s="14"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A111" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B75" s="7"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="7"/>
-      <c r="E75" s="7"/>
-      <c r="F75" s="7"/>
-      <c r="G75" s="7"/>
-      <c r="H75" s="7"/>
-      <c r="I75" s="8"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A76" s="6"/>
-      <c r="B76" s="7" t="s">
+      <c r="B111" s="7"/>
+      <c r="C111" s="7"/>
+      <c r="D111" s="7"/>
+      <c r="E111" s="7"/>
+      <c r="F111" s="7"/>
+      <c r="G111" s="7"/>
+      <c r="H111" s="7"/>
+      <c r="I111" s="8"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A112" s="6"/>
+      <c r="B112" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C76" s="7"/>
-      <c r="D76" s="7"/>
-      <c r="E76" s="7"/>
-      <c r="F76" s="7"/>
-      <c r="G76" s="7"/>
-      <c r="H76" s="7"/>
-      <c r="I76" s="8"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A77" s="6"/>
-      <c r="B77" s="7" t="s">
+      <c r="C112" s="7"/>
+      <c r="D112" s="7"/>
+      <c r="E112" s="7"/>
+      <c r="F112" s="7"/>
+      <c r="G112" s="7"/>
+      <c r="H112" s="7"/>
+      <c r="I112" s="8"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A113" s="6"/>
+      <c r="B113" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C77" s="7"/>
-      <c r="D77" s="7"/>
-      <c r="E77" s="7"/>
-      <c r="F77" s="7"/>
-      <c r="G77" s="7"/>
-      <c r="H77" s="7"/>
-      <c r="I77" s="8"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A78" s="6" t="s">
+      <c r="C113" s="7"/>
+      <c r="D113" s="7"/>
+      <c r="E113" s="7"/>
+      <c r="F113" s="7"/>
+      <c r="G113" s="7"/>
+      <c r="H113" s="7"/>
+      <c r="I113" s="8"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A114" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B78" s="7"/>
-      <c r="C78" s="7"/>
-      <c r="D78" s="7"/>
-      <c r="E78" s="7"/>
-      <c r="F78" s="7"/>
-      <c r="G78" s="7"/>
-      <c r="H78" s="7"/>
-      <c r="I78" s="8"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="16" t="s">
+      <c r="B114" s="7"/>
+      <c r="C114" s="7"/>
+      <c r="D114" s="7"/>
+      <c r="E114" s="7"/>
+      <c r="F114" s="7"/>
+      <c r="G114" s="7"/>
+      <c r="H114" s="7"/>
+      <c r="I114" s="8"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A115" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B79" s="7"/>
-      <c r="C79" s="7"/>
-      <c r="D79" s="7"/>
-      <c r="E79" s="7"/>
-      <c r="F79" s="7"/>
-      <c r="G79" s="7"/>
-      <c r="H79" s="7"/>
-      <c r="I79" s="8"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A80" s="16"/>
-      <c r="B80" s="7"/>
-      <c r="C80" s="7"/>
-      <c r="D80" s="7"/>
-      <c r="E80" s="7"/>
-      <c r="F80" s="7"/>
-      <c r="G80" s="7"/>
-      <c r="H80" s="7"/>
-      <c r="I80" s="8"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A81" s="17" t="s">
+      <c r="B115" s="7"/>
+      <c r="C115" s="7"/>
+      <c r="D115" s="7"/>
+      <c r="E115" s="7"/>
+      <c r="F115" s="7"/>
+      <c r="G115" s="7"/>
+      <c r="H115" s="7"/>
+      <c r="I115" s="8"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A116" s="16"/>
+      <c r="B116" s="7"/>
+      <c r="C116" s="7"/>
+      <c r="D116" s="7"/>
+      <c r="E116" s="7"/>
+      <c r="F116" s="7"/>
+      <c r="G116" s="7"/>
+      <c r="H116" s="7"/>
+      <c r="I116" s="8"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A117" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B81" s="10"/>
-      <c r="C81" s="10"/>
-      <c r="D81" s="10"/>
-      <c r="E81" s="10"/>
-      <c r="F81" s="10"/>
-      <c r="G81" s="10"/>
-      <c r="H81" s="10"/>
-      <c r="I81" s="11"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A82" s="7"/>
-      <c r="B82" s="7"/>
-      <c r="C82" s="7"/>
-      <c r="D82" s="7"/>
-      <c r="E82" s="7"/>
-      <c r="F82" s="7"/>
-      <c r="G82" s="7"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" s="1" t="s">
+      <c r="B117" s="10"/>
+      <c r="C117" s="10"/>
+      <c r="D117" s="10"/>
+      <c r="E117" s="10"/>
+      <c r="F117" s="10"/>
+      <c r="G117" s="10"/>
+      <c r="H117" s="10"/>
+      <c r="I117" s="11"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A118" s="7"/>
+      <c r="B118" s="7"/>
+      <c r="C118" s="7"/>
+      <c r="D118" s="7"/>
+      <c r="E118" s="7"/>
+      <c r="F118" s="7"/>
+      <c r="G118" s="7"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A120" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2326,47 +3125,47 @@
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
-    <col min="3" max="4" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.08984375" customWidth="1"/>
+    <col min="2" max="2" width="13.90625" customWidth="1"/>
+    <col min="3" max="4" width="11.90625" customWidth="1"/>
     <col min="5" max="5" width="13" style="18" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" style="18" customWidth="1"/>
+    <col min="6" max="6" width="14.54296875" style="18" customWidth="1"/>
     <col min="7" max="7" width="13" style="18" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.6328125" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>44238</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="33"/>
       <c r="B5" s="34"/>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="F5" s="37"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="24"/>
       <c r="H5" s="34"/>
       <c r="I5" s="35"/>
     </row>
-    <row r="6" spans="1:9" s="22" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" s="22" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="19" t="s">
         <v>0</v>
       </c>
@@ -2379,10 +3178,10 @@
       <c r="D6" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="38" t="s">
+      <c r="E6" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="36" t="s">
         <v>54</v>
       </c>
       <c r="G6" s="20" t="s">
@@ -2395,7 +3194,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>3</v>
       </c>
@@ -2425,7 +3224,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7">
@@ -2451,7 +3250,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7">
@@ -2477,7 +3276,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="9"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10">
@@ -2503,7 +3302,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
         <v>15</v>
       </c>
@@ -2533,7 +3332,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7">
@@ -2559,7 +3358,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7">
@@ -2585,7 +3384,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="9"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10">
@@ -2611,7 +3410,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>12</v>
       </c>
@@ -2641,7 +3440,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7">
@@ -2667,7 +3466,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7">
@@ -2693,7 +3492,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="9"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10">
@@ -2719,7 +3518,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>13</v>
       </c>
@@ -2749,7 +3548,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7">
@@ -2775,7 +3574,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7">
@@ -2801,7 +3600,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10">
@@ -2827,7 +3626,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
         <v>56</v>
       </c>
@@ -2860,7 +3659,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="6"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7">
@@ -2889,7 +3688,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="6"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7">
@@ -2918,7 +3717,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="9"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10">
@@ -2947,7 +3746,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
         <v>14</v>
       </c>
@@ -2977,7 +3776,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="6"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7">
@@ -3003,7 +3802,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="6"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7">
@@ -3029,7 +3828,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="9"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10">
@@ -3055,7 +3854,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
         <v>17</v>
       </c>
@@ -3085,7 +3884,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="6"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7">
@@ -3111,7 +3910,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="6"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7">
@@ -3137,7 +3936,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="9"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10">
@@ -3163,7 +3962,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
         <v>18</v>
       </c>
@@ -3193,7 +3992,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="6"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7">
@@ -3219,7 +4018,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="6"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7">
@@ -3245,7 +4044,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="9"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10">
@@ -3271,7 +4070,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
         <v>64</v>
       </c>
@@ -3294,11 +4093,11 @@
         <f>AVERAGE(H7,H11,H23,H27,H31,H35)</f>
         <v>0.80986883115168939</v>
       </c>
-      <c r="I39" s="40">
+      <c r="I39" s="38">
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="6"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7">
@@ -3317,11 +4116,11 @@
         <f t="shared" si="3"/>
         <v>1.001768977271559</v>
       </c>
-      <c r="I40" s="39">
+      <c r="I40" s="37">
         <v>0.5</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="6"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7">
@@ -3340,11 +4139,11 @@
         <f t="shared" si="3"/>
         <v>0.99314137272755476</v>
       </c>
-      <c r="I41" s="39">
+      <c r="I41" s="37">
         <v>0.5</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="9"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10">
@@ -3363,11 +4162,11 @@
         <f t="shared" si="3"/>
         <v>0.76213011108698803</v>
       </c>
-      <c r="I42" s="41">
+      <c r="I42" s="39">
         <v>0.5</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -3378,7 +4177,7 @@
       <c r="H43" s="29"/>
       <c r="I43" s="7"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -3389,7 +4188,7 @@
       <c r="H44" s="29"/>
       <c r="I44" s="7"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="33" t="s">
         <v>60</v>
       </c>
@@ -3403,17 +4202,17 @@
       <c r="I47" s="34"/>
       <c r="J47" s="35"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>62</v>
       </c>

</xml_diff>